<commit_message>
Working on static path
</commit_message>
<xml_diff>
--- a/ACI_Builder/EPG_Input.xlsx
+++ b/ACI_Builder/EPG_Input.xlsx
@@ -38,9 +38,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Static_Path</t>
-  </si>
-  <si>
     <t>VMM_Domain</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>E7_NETAPP</t>
   </si>
   <si>
-    <t>e7_NETAPP-A_VPC</t>
-  </si>
-  <si>
     <t>acitoolkit</t>
   </si>
   <si>
@@ -162,6 +156,12 @@
   </si>
   <si>
     <t>443</t>
+  </si>
+  <si>
+    <t>Static_Path 1/101/1/13</t>
+  </si>
+  <si>
+    <t>1/201/1/8</t>
   </si>
 </sst>
 </file>
@@ -488,13 +488,15 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="6" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="20.5" customWidth="1"/>
     <col min="8" max="8" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" customWidth="1"/>
@@ -502,34 +504,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -537,71 +539,71 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F2" s="2">
         <v>800</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
         <v>7</v>
-      </c>
-      <c r="I3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -609,82 +611,82 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
       <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" t="s">
-        <v>26</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added statements to differentiate between single static port paths and VPC paths
</commit_message>
<xml_diff>
--- a/ACI_Builder/EPG_Input.xlsx
+++ b/ACI_Builder/EPG_Input.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="480" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TenantConfig" sheetId="1" r:id="rId1"/>
+    <sheet name="Physical Paths" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Create_EPG</t>
   </si>
@@ -161,17 +162,48 @@
     <t>Static_Path 1/101/1/13</t>
   </si>
   <si>
-    <t>1/201/1/8</t>
+    <t>VPC</t>
+  </si>
+  <si>
+    <t>e7f50bigip01</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>201-202</t>
+  </si>
+  <si>
+    <t>24,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,8 +232,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -209,7 +247,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -487,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -548,7 +592,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" s="2">
         <v>800</v>
@@ -691,5 +735,49 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added the ability to attach VMM domain to EPGs
</commit_message>
<xml_diff>
--- a/ACI_Builder/EPG_Input.xlsx
+++ b/ACI_Builder/EPG_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TenantConfig" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Contract</t>
   </si>
   <si>
-    <t>e7vmw1vic02</t>
-  </si>
-  <si>
     <t>e7_L3_Out</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>encap_vlan</t>
   </si>
   <si>
-    <t>E7_NETAPP</t>
-  </si>
-  <si>
     <t>acitoolkit</t>
   </si>
   <si>
@@ -159,9 +153,6 @@
     <t>443</t>
   </si>
   <si>
-    <t>Static_Path 1/101/1/13</t>
-  </si>
-  <si>
     <t>VPC</t>
   </si>
   <si>
@@ -178,6 +169,15 @@
   </si>
   <si>
     <t>24,</t>
+  </si>
+  <si>
+    <t>Static_Path 1/101/1/13 or VPC name</t>
+  </si>
+  <si>
+    <t>e7vmw1_Data</t>
+  </si>
+  <si>
+    <t>e7_f5_phys</t>
   </si>
 </sst>
 </file>
@@ -241,11 +241,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -531,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,24 +549,24 @@
     <col min="9" max="9" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
+      <c r="E1" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
@@ -575,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -583,71 +586,71 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="2">
+        <v>740</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="2">
-        <v>800</v>
-      </c>
-      <c r="G2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
-      </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
         <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -655,82 +658,82 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="I8" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>24</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -743,7 +746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -756,24 +759,24 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>